<commit_message>
add PMS100 and DCA, reorganized script structure
</commit_message>
<xml_diff>
--- a/Resources/Validation.xlsx
+++ b/Resources/Validation.xlsx
@@ -46,7 +46,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -64,16 +64,20 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,19 +407,19 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4">
-        <v>42956.791666666664</v>
+      <c r="D1" s="6">
+        <v>42957.791666666664</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel spreadsheet with prefilled data
</commit_message>
<xml_diff>
--- a/Resources/Validation.xlsx
+++ b/Resources/Validation.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Invoice No</t>
   </si>
@@ -23,13 +23,151 @@
   </si>
   <si>
     <t>Customer PO</t>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>Shipment Date</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Whs</t>
+  </si>
+  <si>
+    <t>Deliver Number</t>
+  </si>
+  <si>
+    <t>Delivery Account</t>
+  </si>
+  <si>
+    <t>Pay Account</t>
+  </si>
+  <si>
+    <t>Pay Address</t>
+  </si>
+  <si>
+    <t>Delivery Address</t>
+  </si>
+  <si>
+    <t>Payment Terms</t>
+  </si>
+  <si>
+    <t>Delivery Method</t>
+  </si>
+  <si>
+    <t>Payment Discount</t>
+  </si>
+  <si>
+    <t>Strap Style</t>
+  </si>
+  <si>
+    <t>Location 1</t>
+  </si>
+  <si>
+    <t>Personalization1</t>
+  </si>
+  <si>
+    <t>Pers 1-Lettering</t>
+  </si>
+  <si>
+    <t>US-Gear-06</t>
+  </si>
+  <si>
+    <t>06Y</t>
+  </si>
+  <si>
+    <t>US00023553</t>
+  </si>
+  <si>
+    <t>US00025065</t>
+  </si>
+  <si>
+    <t>ATTN GIL M GUSWEILER</t>
+  </si>
+  <si>
+    <t>6501 KENWOOD RD</t>
+  </si>
+  <si>
+    <t>CINCINNATI OH 45243-2315</t>
+  </si>
+  <si>
+    <t>KENWOOD COUNTRY CLUB INC</t>
+  </si>
+  <si>
+    <t>KENWOOD COUNTRY CLUB</t>
+  </si>
+  <si>
+    <t>Net 60 Days</t>
+  </si>
+  <si>
+    <t>FedEx Ground</t>
+  </si>
+  <si>
+    <t>2% 30 Days</t>
+  </si>
+  <si>
+    <t>Double Strap (Standard)</t>
+  </si>
+  <si>
+    <t>Apparel Pocket L1</t>
+  </si>
+  <si>
+    <t>My custom personalization</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Pers 1-Color</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Item Codes</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-016</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-041</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-226</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-246</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-3</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-4</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-423</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-428</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-6</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Bag S&amp;H Charge ($5) - Level 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -61,29 +199,25 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -376,28 +510,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="11.6328125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="9.81640625" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -407,19 +560,188 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6">
-        <v>42957.791666666664</v>
-      </c>
-    </row>
-    <row r="2">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>3013684370</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>904492469</v>
+      </c>
+      <c r="D2" s="2">
+        <v>42937</v>
+      </c>
+      <c r="E2" s="2">
+        <v>42937</v>
+      </c>
+      <c r="F2" s="2">
+        <v>42934</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>13117639</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" t="s">
         <v>33</v>
       </c>
-      <c r="C2">
-        <v>75</v>
+      <c r="S2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move some misplaced images and add schedule number generation function with excel counter backing
</commit_message>
<xml_diff>
--- a/Resources/Validation.xlsx
+++ b/Resources/Validation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -166,8 +167,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,19 +206,14 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -510,47 +506,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="12.5703125" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.42578125" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="12" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="14.28515625" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="10.7109375" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="4.85546875" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="15.28515625" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="16.140625" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="28.42578125" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="25.28515625" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="14.85546875" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="16" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="17.28515625" bestFit="true" customWidth="true"/>
+    <col min="16" max="16" width="22.5703125" bestFit="true" customWidth="true"/>
+    <col min="17" max="17" width="16.85546875" bestFit="true" customWidth="true"/>
+    <col min="18" max="18" width="25.140625" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="15.140625" bestFit="true" customWidth="true"/>
+    <col min="20" max="20" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="21" max="21" width="13.42578125" bestFit="true" customWidth="true"/>
+    <col min="22" max="22" width="27" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -618,7 +614,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2">
         <v>3013684370</v>
       </c>
@@ -686,7 +682,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="K3" t="s">
         <v>23</v>
       </c>
@@ -697,7 +693,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="K4" t="s">
         <v>24</v>
       </c>
@@ -708,7 +704,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="K5" t="s">
         <v>25</v>
       </c>
@@ -719,27 +715,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="U6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="U7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="U8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="U9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="U10" t="s">
         <v>46</v>
       </c>
@@ -748,4 +744,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix packing status checking, some better pictures
</commit_message>
<xml_diff>
--- a/Resources/Validation.xlsx
+++ b/Resources/Validation.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>Invoice No</t>
   </si>
@@ -162,6 +163,114 @@
   </si>
   <si>
     <t>Bag S&amp;H Charge ($5) - Level 2</t>
+  </si>
+  <si>
+    <t>Schedule Number Counter</t>
+  </si>
+  <si>
+    <t>Data Recorder Index</t>
+  </si>
+  <si>
+    <t>CONumber</t>
+  </si>
+  <si>
+    <t>MONumber</t>
+  </si>
+  <si>
+    <t>ScheduleNumber</t>
+  </si>
+  <si>
+    <t>DeliveryNumber</t>
+  </si>
+  <si>
+    <t>3013691711</t>
+  </si>
+  <si>
+    <t>1000004200</t>
+  </si>
+  <si>
+    <t>13141381</t>
+  </si>
+  <si>
+    <t>3013691714</t>
+  </si>
+  <si>
+    <t>1000004203</t>
+  </si>
+  <si>
+    <t>13141387</t>
+  </si>
+  <si>
+    <t>3013691715</t>
+  </si>
+  <si>
+    <t>1000004204</t>
+  </si>
+  <si>
+    <t>13141389</t>
+  </si>
+  <si>
+    <t>3013691716</t>
+  </si>
+  <si>
+    <t>1000004205</t>
+  </si>
+  <si>
+    <t>13141391</t>
+  </si>
+  <si>
+    <t>3013691717</t>
+  </si>
+  <si>
+    <t>1000004206</t>
+  </si>
+  <si>
+    <t>13141393</t>
+  </si>
+  <si>
+    <t>3013691718</t>
+  </si>
+  <si>
+    <t>1000004207</t>
+  </si>
+  <si>
+    <t>13141395</t>
+  </si>
+  <si>
+    <t>3013691730</t>
+  </si>
+  <si>
+    <t>1000004218</t>
+  </si>
+  <si>
+    <t>13141496</t>
+  </si>
+  <si>
+    <t>3013691731</t>
+  </si>
+  <si>
+    <t>1000004219</t>
+  </si>
+  <si>
+    <t>13141498</t>
+  </si>
+  <si>
+    <t>3013691732</t>
+  </si>
+  <si>
+    <t>1000004220</t>
+  </si>
+  <si>
+    <t>13141500</t>
+  </si>
+  <si>
+    <t>3013691733</t>
+  </si>
+  <si>
+    <t>1000004221</t>
+  </si>
+  <si>
+    <t>13141502</t>
   </si>
 </sst>
 </file>
@@ -748,15 +857,206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="true" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>95</v>
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="11.42578125" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="16.5703125" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="15.85546875" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>21708102017</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3">
+        <v>22008102017</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4">
+        <v>22108102017</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5">
+        <v>22208102017</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6">
+        <v>22308102017</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7">
+        <v>22408102017</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>22608102017</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9">
+        <v>22708102017</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>22808102017</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11">
+        <v>22908102017</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made to PO receiving
</commit_message>
<xml_diff>
--- a/Resources/Validation.xlsx
+++ b/Resources/Validation.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
   <si>
     <t>Invoice No</t>
   </si>
@@ -271,14 +272,25 @@
   </si>
   <si>
     <t>13141502</t>
+  </si>
+  <si>
+    <t>PONumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -313,16 +325,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -369,7 +387,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -421,7 +439,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -615,47 +633,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="12.5703125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.42578125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="12" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="14.28515625" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="10.7109375" bestFit="true" customWidth="true"/>
-    <col min="7" max="7" width="4.85546875" bestFit="true" customWidth="true"/>
-    <col min="8" max="8" width="15.28515625" bestFit="true" customWidth="true"/>
-    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
-    <col min="10" max="10" width="16.140625" bestFit="true" customWidth="true"/>
-    <col min="11" max="11" width="28.42578125" bestFit="true" customWidth="true"/>
-    <col min="12" max="12" width="25.28515625" bestFit="true" customWidth="true"/>
-    <col min="13" max="13" width="14.85546875" bestFit="true" customWidth="true"/>
-    <col min="14" max="14" width="16" bestFit="true" customWidth="true"/>
-    <col min="15" max="15" width="17.28515625" bestFit="true" customWidth="true"/>
-    <col min="16" max="16" width="22.5703125" bestFit="true" customWidth="true"/>
-    <col min="17" max="17" width="16.85546875" bestFit="true" customWidth="true"/>
-    <col min="18" max="18" width="25.140625" bestFit="true" customWidth="true"/>
-    <col min="19" max="19" width="15.140625" bestFit="true" customWidth="true"/>
-    <col min="20" max="20" width="11.7109375" bestFit="true" customWidth="true"/>
-    <col min="21" max="21" width="13.42578125" bestFit="true" customWidth="true"/>
-    <col min="22" max="22" width="27" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -723,7 +741,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3013684370</v>
       </c>
@@ -791,7 +809,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
         <v>23</v>
       </c>
@@ -802,7 +820,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
         <v>24</v>
       </c>
@@ -813,7 +831,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
         <v>25</v>
       </c>
@@ -824,27 +842,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U10" t="s">
         <v>46</v>
       </c>
@@ -856,19 +874,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -876,7 +894,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -890,22 +908,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="11.42578125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="16.5703125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="15.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -919,7 +937,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -933,7 +951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -947,7 +965,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -961,7 +979,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -975,7 +993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -989,7 +1007,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1003,7 +1021,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1017,7 +1035,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -1031,7 +1049,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1045,7 +1063,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -1062,4 +1080,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1198965</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1090489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1090490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1090492</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1090492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1090494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1090494</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1090495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1090496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1090496</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added on 19sep 2017
</commit_message>
<xml_diff>
--- a/Resources/Validation.xlsx
+++ b/Resources/Validation.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>Invoice No</t>
   </si>
@@ -271,13 +272,25 @@
   </si>
   <si>
     <t>13141502</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>PWD</t>
+  </si>
+  <si>
+    <t>Ajenkins</t>
+  </si>
+  <si>
+    <t>Acushnet#1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,14 +328,19 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -369,7 +387,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -421,7 +439,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -622,40 +640,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="12.5703125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.42578125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="12" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="14.28515625" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="10.7109375" bestFit="true" customWidth="true"/>
-    <col min="7" max="7" width="4.85546875" bestFit="true" customWidth="true"/>
-    <col min="8" max="8" width="15.28515625" bestFit="true" customWidth="true"/>
-    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
-    <col min="10" max="10" width="16.140625" bestFit="true" customWidth="true"/>
-    <col min="11" max="11" width="28.42578125" bestFit="true" customWidth="true"/>
-    <col min="12" max="12" width="25.28515625" bestFit="true" customWidth="true"/>
-    <col min="13" max="13" width="14.85546875" bestFit="true" customWidth="true"/>
-    <col min="14" max="14" width="16" bestFit="true" customWidth="true"/>
-    <col min="15" max="15" width="17.28515625" bestFit="true" customWidth="true"/>
-    <col min="16" max="16" width="22.5703125" bestFit="true" customWidth="true"/>
-    <col min="17" max="17" width="16.85546875" bestFit="true" customWidth="true"/>
-    <col min="18" max="18" width="25.140625" bestFit="true" customWidth="true"/>
-    <col min="19" max="19" width="15.140625" bestFit="true" customWidth="true"/>
-    <col min="20" max="20" width="11.7109375" bestFit="true" customWidth="true"/>
-    <col min="21" max="21" width="13.42578125" bestFit="true" customWidth="true"/>
-    <col min="22" max="22" width="27" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -723,7 +741,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3013684370</v>
       </c>
@@ -791,7 +809,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
         <v>23</v>
       </c>
@@ -802,7 +820,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
         <v>24</v>
       </c>
@@ -813,7 +831,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
         <v>25</v>
       </c>
@@ -824,27 +842,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U10" t="s">
         <v>46</v>
       </c>
@@ -856,19 +874,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -876,7 +894,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -890,22 +908,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="11.42578125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="16.5703125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="15.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -919,7 +937,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -933,7 +951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -947,7 +965,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -961,7 +979,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -975,7 +993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -989,7 +1007,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1003,7 +1021,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1017,7 +1035,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -1031,7 +1049,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1045,7 +1063,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -1057,6 +1075,37 @@
       </c>
       <c r="D11" t="s">
         <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made to script4
</commit_message>
<xml_diff>
--- a/Resources/Validation.xlsx
+++ b/Resources/Validation.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>Invoice No</t>
   </si>
@@ -271,16 +272,42 @@
   </si>
   <si>
     <t>13141502</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ajenkins</t>
+  </si>
+  <si>
+    <t>Acushnet#1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,16 +340,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -369,7 +404,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -421,7 +456,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -615,47 +650,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="12.5703125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.42578125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="12" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="14.28515625" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="10.7109375" bestFit="true" customWidth="true"/>
-    <col min="7" max="7" width="4.85546875" bestFit="true" customWidth="true"/>
-    <col min="8" max="8" width="15.28515625" bestFit="true" customWidth="true"/>
-    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
-    <col min="10" max="10" width="16.140625" bestFit="true" customWidth="true"/>
-    <col min="11" max="11" width="28.42578125" bestFit="true" customWidth="true"/>
-    <col min="12" max="12" width="25.28515625" bestFit="true" customWidth="true"/>
-    <col min="13" max="13" width="14.85546875" bestFit="true" customWidth="true"/>
-    <col min="14" max="14" width="16" bestFit="true" customWidth="true"/>
-    <col min="15" max="15" width="17.28515625" bestFit="true" customWidth="true"/>
-    <col min="16" max="16" width="22.5703125" bestFit="true" customWidth="true"/>
-    <col min="17" max="17" width="16.85546875" bestFit="true" customWidth="true"/>
-    <col min="18" max="18" width="25.140625" bestFit="true" customWidth="true"/>
-    <col min="19" max="19" width="15.140625" bestFit="true" customWidth="true"/>
-    <col min="20" max="20" width="11.7109375" bestFit="true" customWidth="true"/>
-    <col min="21" max="21" width="13.42578125" bestFit="true" customWidth="true"/>
-    <col min="22" max="22" width="27" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -723,7 +758,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3013684370</v>
       </c>
@@ -791,7 +826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
         <v>23</v>
       </c>
@@ -802,7 +837,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
         <v>24</v>
       </c>
@@ -813,7 +848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
         <v>25</v>
       </c>
@@ -824,27 +859,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U10" t="s">
         <v>46</v>
       </c>
@@ -856,19 +891,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -876,7 +911,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -890,22 +925,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="11.42578125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="16.5703125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="15.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -919,7 +954,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -933,7 +968,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -947,7 +982,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -961,7 +996,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -975,7 +1010,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -989,7 +1024,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1003,7 +1038,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1017,7 +1052,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -1031,7 +1066,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1045,7 +1080,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -1058,6 +1093,54 @@
       <c r="D11" t="s">
         <v>84</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>